<commit_message>
thiet ke man hinh - 5
</commit_message>
<xml_diff>
--- a/03.Design/ScreenV1.xlsx
+++ b/03.Design/ScreenV1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155"/>
   </bookViews>
   <sheets>
     <sheet name="Top" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>List item</t>
   </si>
@@ -46,15 +46,6 @@
     <t>2. Mục 2 cho phép nhập mật khẩu, để mật khẩu dạng sao để bảo mật</t>
   </si>
   <si>
-    <t>1. Chọn mục 1 hiện bàn phím để nhập</t>
-  </si>
-  <si>
-    <t>2. Chọn mục 2 hiện bàn phím để nhập</t>
-  </si>
-  <si>
-    <t>3. Sau khi bấm nút ở mục 3:</t>
-  </si>
-  <si>
     <t>Error message</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>1. Chọn mục 1,2,6 hiện bàn phím để nhập</t>
   </si>
   <si>
-    <t>3. Thiếu trường nào thì báo lỗi ở trường đấy</t>
-  </si>
-  <si>
     <t>6. EditText nhập mật khẩu</t>
   </si>
   <si>
@@ -136,24 +124,12 @@
     <t>- nếu nhập đúng thì chuyển sang màn hình Mypage</t>
   </si>
   <si>
-    <t>1. Chạm vào mục 1 sẽ chuyển sang màn hình Shinki</t>
-  </si>
-  <si>
-    <t>2. Chạm vào mục 2 sẽ chuyển sang màn hình Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Chạm vào mục 3 sẽ chuyển sang màn hình Reminder </t>
-  </si>
-  <si>
     <t>- nếu nhập đúng đủ thì đẩy dữ liệu ở các trường lên server kiểm tra:</t>
   </si>
   <si>
     <t>+ tài khoản đã tại thì đẩy sang màn hình Error2</t>
   </si>
   <si>
-    <t>+ tài khoản chưa tồn tại thì cập nhật trên server và đẩy sang màn hình Mypage</t>
-  </si>
-  <si>
     <t>- nếu nhập thiếu hoặc sai thì đẩy sang màn hình Error1</t>
   </si>
   <si>
@@ -226,9 +202,6 @@
     <t>11. Button đăng ký</t>
   </si>
   <si>
-    <t>1.TextView mô tả</t>
-  </si>
-  <si>
     <t>1. Mục 2 cho phép nhập first name, kiểm tra không cho để trống</t>
   </si>
   <si>
@@ -268,18 +241,9 @@
     <t>2. Muốn đăng ký thành công phải chấp nhận điều khoản và tích vào mục 10</t>
   </si>
   <si>
-    <t>- nếu nhập thiếu thì báo lỗi 2</t>
-  </si>
-  <si>
-    <t>2. Thiếu trường nào thì báo lỗi thiếu trường đấy</t>
-  </si>
-  <si>
     <t>1. TextView mô tả</t>
   </si>
   <si>
-    <t xml:space="preserve">2. TextView thông báo nhập thiếu </t>
-  </si>
-  <si>
     <t xml:space="preserve">3. Button trở về </t>
   </si>
   <si>
@@ -356,6 +320,33 @@
   </si>
   <si>
     <t xml:space="preserve">2. Sau khi chạm vào mục 6 thì chuyển sang màn hình Edit </t>
+  </si>
+  <si>
+    <t>2. Chạm vào mục 3 sẽ chuyển sang màn hình Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Chạm vào mục 4 sẽ chuyển sang màn hình Reminder </t>
+  </si>
+  <si>
+    <t>1. Chạm vào mục 2 sẽ chuyển sang màn hình Registration</t>
+  </si>
+  <si>
+    <t>1. Chọn mục 2 hiện bàn phím để nhập</t>
+  </si>
+  <si>
+    <t>2. Chọn mục 3 hiện bàn phím để nhập</t>
+  </si>
+  <si>
+    <t>3. Sau khi bấm nút ở mục 4:</t>
+  </si>
+  <si>
+    <t>- nếu nhập thiếu thì đẩy sang màn hình Error1</t>
+  </si>
+  <si>
+    <t>2. TextView thông báo nhập thiếu trường</t>
+  </si>
+  <si>
+    <t>+ tài khoản chưa tồn tại thì cập nhật trên server và đẩy sang màn hình Registration_info</t>
   </si>
 </sst>
 </file>
@@ -4686,8 +4677,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4719,7 +4710,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -4730,7 +4721,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -4741,7 +4732,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -4752,7 +4743,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -4801,7 +4792,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -4812,7 +4803,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -4823,7 +4814,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -4842,7 +4833,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="H15" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -4856,7 +4847,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="H16" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -5049,8 +5040,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5085,7 +5076,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -5096,7 +5087,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5107,7 +5098,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5118,7 +5109,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5148,7 +5139,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5189,7 +5180,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="H13" s="2" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -5200,7 +5191,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="H14" s="2" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -5211,7 +5202,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -5222,7 +5213,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="I16" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -5233,7 +5224,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="I17" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -5252,7 +5243,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -5266,7 +5257,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="H20" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -5428,8 +5419,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5464,7 +5455,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -5475,7 +5466,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -5486,7 +5477,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -5497,7 +5488,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -5508,7 +5499,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -5519,7 +5510,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -5530,7 +5521,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5541,7 +5532,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -5552,7 +5543,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -5563,7 +5554,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -5574,7 +5565,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="H13" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -5604,7 +5595,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="H16" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -5615,7 +5606,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="H17" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -5626,7 +5617,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -5637,7 +5628,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -5648,7 +5639,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="H20" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -5659,7 +5650,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="H21" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -5670,7 +5661,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="H22" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -5681,7 +5672,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="H23" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -5692,7 +5683,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="H24" s="2" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -5722,7 +5713,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="H27" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -5733,7 +5724,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="H28" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -5744,7 +5735,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="H29" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -5755,7 +5746,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="I30" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -5766,7 +5757,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="I31" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -5777,7 +5768,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="J32" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -5788,7 +5779,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="J33" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -5807,7 +5798,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="H35" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
@@ -5824,7 +5815,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="H36" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
@@ -5841,7 +5832,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="H37" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
@@ -5857,9 +5848,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="H38" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
@@ -5880,7 +5869,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5915,7 +5904,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -5926,7 +5915,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -5937,7 +5926,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -5948,7 +5937,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -5959,7 +5948,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -5970,7 +5959,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -5981,7 +5970,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -5992,7 +5981,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -6003,7 +5992,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -6033,7 +6022,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="H14" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -6044,7 +6033,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -6055,7 +6044,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="H16" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -6066,7 +6055,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="H17" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -6077,7 +6066,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -6088,7 +6077,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -6099,7 +6088,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="H20" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -6110,7 +6099,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="H21" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -6140,7 +6129,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="H24" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -6151,7 +6140,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="H25" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -6162,7 +6151,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="H26" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -6173,7 +6162,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="I27" s="2" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -6184,7 +6173,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="I28" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -6203,7 +6192,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="H30" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -6220,7 +6209,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="H31" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -6236,9 +6225,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="H32" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -6306,8 +6293,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6342,7 +6329,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -6353,7 +6340,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6364,7 +6351,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -6413,7 +6400,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -6432,7 +6419,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -6446,7 +6433,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="H13" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -6700,7 +6687,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -6711,7 +6698,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6722,7 +6709,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -6733,7 +6720,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -6782,7 +6769,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -6793,7 +6780,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -6812,7 +6799,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="H14" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -6826,7 +6813,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="H15" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -7028,7 +7015,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -7064,7 +7051,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -7075,7 +7062,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -7086,7 +7073,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -7097,7 +7084,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -7108,7 +7095,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7138,7 +7125,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -7168,7 +7155,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="H13" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -7179,7 +7166,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="I14" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -7190,7 +7177,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="I15" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -7209,7 +7196,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="H17" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -7223,7 +7210,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -7237,7 +7224,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -7406,7 +7393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
@@ -7442,7 +7429,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -7453,7 +7440,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -7464,7 +7451,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -7475,7 +7462,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -7486,7 +7473,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -7497,7 +7484,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -7508,7 +7495,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -7519,7 +7506,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -7568,7 +7555,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -7579,7 +7566,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="H16" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -7598,7 +7585,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -7612,7 +7599,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -7785,7 +7772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -7821,7 +7808,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -7832,7 +7819,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -7843,7 +7830,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -7854,7 +7841,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -7865,7 +7852,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="H7" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -7876,7 +7863,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -7925,7 +7912,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="H13" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -7936,7 +7923,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="H14" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -7963,7 +7950,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="H17" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -7977,7 +7964,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="H18" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>

</xml_diff>

<commit_message>
update screen.xls + màn hình Top,Login,Regis,Reminder,RegisInfo
</commit_message>
<xml_diff>
--- a/03.Design/ScreenV1.xlsx
+++ b/03.Design/ScreenV1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\03.Design\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10068" windowHeight="4152" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Top" sheetId="1" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <sheet name="Registration_info" sheetId="9" r:id="rId8"/>
     <sheet name="Mypage" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="147">
   <si>
     <t>List item</t>
   </si>
@@ -362,13 +357,124 @@
   </si>
   <si>
     <t>Handle event (API INFORMATION)</t>
+  </si>
+  <si>
+    <t>お名前</t>
+  </si>
+  <si>
+    <t>山田花子</t>
+  </si>
+  <si>
+    <t>生年月日</t>
+  </si>
+  <si>
+    <t>2008年12月31日</t>
+  </si>
+  <si>
+    <t>学校名</t>
+  </si>
+  <si>
+    <t>私立〇x〇x小学校</t>
+  </si>
+  <si>
+    <t>メールアドレス</t>
+  </si>
+  <si>
+    <t>hanako_yamada@gmail.com</t>
+  </si>
+  <si>
+    <t>パスワード</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>この画面をスクシヨで保存して下さい。</t>
+  </si>
+  <si>
+    <t>アプリを利用する</t>
+  </si>
+  <si>
+    <t>ログイン</t>
+  </si>
+  <si>
+    <t>山田</t>
+  </si>
+  <si>
+    <t>花子</t>
+  </si>
+  <si>
+    <t>年</t>
+  </si>
+  <si>
+    <t>月</t>
+  </si>
+  <si>
+    <t>日</t>
+  </si>
+  <si>
+    <t>メールアドレス（任意）</t>
+  </si>
+  <si>
+    <t>パスワ一ド</t>
+  </si>
+  <si>
+    <t>英数字〇桁以上</t>
+  </si>
+  <si>
+    <t>本サービスをご利用するには利用規約への同意が必要です。</t>
+  </si>
+  <si>
+    <t>利用規約に同意する</t>
+  </si>
+  <si>
+    <t>登録</t>
+  </si>
+  <si>
+    <t>入力項目の誤りがあります。</t>
+  </si>
+  <si>
+    <t>có 1 từ không copy paste được…</t>
+  </si>
+  <si>
+    <t>戻る</t>
+  </si>
+  <si>
+    <t>既に登録しているアカウントです。</t>
+  </si>
+  <si>
+    <t>ログイン情報をお忘れの方はこちら</t>
+  </si>
+  <si>
+    <t>学校の追加</t>
+  </si>
+  <si>
+    <t>変更申請</t>
+  </si>
+  <si>
+    <t>ログイン情報をお忘れの方は、登録のメールアド レスをご入力ください。アドレス宛にログイン情報 を送付いたします。</t>
+  </si>
+  <si>
+    <t>送信</t>
+  </si>
+  <si>
+    <t>2008年12月31日生まれ</t>
+  </si>
+  <si>
+    <t>私立〇x〇x中学校</t>
+  </si>
+  <si>
+    <t>新規登録</t>
+  </si>
+  <si>
+    <t>パスワードをお忘れの方</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +488,15 @@
       <color rgb="FF0070C0"/>
       <name val="Franklin Gothic Medium"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -413,10 +528,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -424,12 +540,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -461,7 +607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEFD6435-6F2F-4713-8C1D-01F286202A46}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEFD6435-6F2F-4713-8C1D-01F286202A46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -511,7 +657,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A51231CA-F271-4783-AE52-345E1CD1AEF9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A51231CA-F271-4783-AE52-345E1CD1AEF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -575,7 +721,7 @@
         <xdr:cNvPr id="7" name="Oval 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5EBBF2B-7E87-4617-842F-B48285C815D7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5EBBF2B-7E87-4617-842F-B48285C815D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -639,7 +785,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{583A63D8-A7BD-4F05-99D4-05EC6BC91597}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{583A63D8-A7BD-4F05-99D4-05EC6BC91597}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -703,7 +849,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC95FF5-321C-444C-A99F-8FD3ADD9DE65}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC95FF5-321C-444C-A99F-8FD3ADD9DE65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -772,7 +918,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{975461AD-EFF4-4921-B0D9-5B565ABA4738}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{975461AD-EFF4-4921-B0D9-5B565ABA4738}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -822,7 +968,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9320DF-144E-46C3-8E38-55D4D17ECDFE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9320DF-144E-46C3-8E38-55D4D17ECDFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -886,7 +1032,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B1E321-A1F9-4BD3-8CB1-1592A2F3C4BF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B1E321-A1F9-4BD3-8CB1-1592A2F3C4BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -950,7 +1096,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2D851E-C16F-48E5-8533-24AD1478B4C3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2D851E-C16F-48E5-8533-24AD1478B4C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1014,7 +1160,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C75007-C588-4A9D-BF3B-5316CC823742}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C75007-C588-4A9D-BF3B-5316CC823742}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1083,7 +1229,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DBDB091-1275-4959-BDAD-72B3659E7C9E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DBDB091-1275-4959-BDAD-72B3659E7C9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1133,7 +1279,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DF8E88-514A-4E06-A148-443346C88D6D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DF8E88-514A-4E06-A148-443346C88D6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1197,7 +1343,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BC0D453-CB71-463E-8BF7-8E37D4013D31}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BC0D453-CB71-463E-8BF7-8E37D4013D31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1261,7 +1407,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5425B5F-D857-4E9E-BD8A-EA921061B9D1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5425B5F-D857-4E9E-BD8A-EA921061B9D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1325,7 +1471,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7938031A-FBA9-4A5B-9617-445B09FC6CBE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7938031A-FBA9-4A5B-9617-445B09FC6CBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1389,7 +1535,7 @@
         <xdr:cNvPr id="7" name="Oval 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23690A45-8B1E-4F72-9AA3-60404569EEEA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23690A45-8B1E-4F72-9AA3-60404569EEEA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1453,7 +1599,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{702F7016-7A7A-4C00-9EF6-E013D3FF1682}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{702F7016-7A7A-4C00-9EF6-E013D3FF1682}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1517,7 +1663,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56EBE8ED-1FA8-442F-B839-4E37F6A411ED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56EBE8ED-1FA8-442F-B839-4E37F6A411ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1581,7 +1727,7 @@
         <xdr:cNvPr id="10" name="Oval 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B13AA4-46D2-41F5-929F-074C2911B948}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87B13AA4-46D2-41F5-929F-074C2911B948}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1645,7 +1791,7 @@
         <xdr:cNvPr id="11" name="Oval 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B957D2-B8B7-4372-A604-60A3BBB26D24}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B957D2-B8B7-4372-A604-60A3BBB26D24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1709,7 +1855,7 @@
         <xdr:cNvPr id="12" name="Oval 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16261078-5B95-45F3-B9C0-FD0C0EA6D25A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16261078-5B95-45F3-B9C0-FD0C0EA6D25A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1773,7 +1919,7 @@
         <xdr:cNvPr id="13" name="Oval 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBE34A34-D141-44D9-963B-21E9E183FF67}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBE34A34-D141-44D9-963B-21E9E183FF67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1842,7 +1988,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03CD8914-F68A-41CE-9AB4-6104F2B57D13}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03CD8914-F68A-41CE-9AB4-6104F2B57D13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1892,7 +2038,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FED1F271-3753-400F-B86B-A4085BCB34B7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FED1F271-3753-400F-B86B-A4085BCB34B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1956,7 +2102,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CB8E740-03D4-4196-A60C-197075BD760E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CB8E740-03D4-4196-A60C-197075BD760E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2020,7 +2166,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19C2FF3-F2BC-4131-9E6F-64CDCF497DB7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19C2FF3-F2BC-4131-9E6F-64CDCF497DB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2084,7 +2230,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A7C3BA-25E3-45A3-A7F5-21BB7A6D9D9E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A7C3BA-25E3-45A3-A7F5-21BB7A6D9D9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2148,7 +2294,7 @@
         <xdr:cNvPr id="7" name="Oval 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42878C0B-C8B1-428C-B6AA-14CC0E639F68}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42878C0B-C8B1-428C-B6AA-14CC0E639F68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2212,7 +2358,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9079DF29-2A19-4701-8FB4-2F27B2832228}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9079DF29-2A19-4701-8FB4-2F27B2832228}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2276,7 +2422,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1A66DC9-F914-4693-AF9E-C9B3DEF0E64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1A66DC9-F914-4693-AF9E-C9B3DEF0E64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2340,7 +2486,7 @@
         <xdr:cNvPr id="10" name="Oval 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF88E0C5-98ED-4ED2-9C57-BA65F23B75D9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF88E0C5-98ED-4ED2-9C57-BA65F23B75D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2404,7 +2550,7 @@
         <xdr:cNvPr id="11" name="Oval 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86CDFB7F-8249-4DC8-9334-19967328EA30}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86CDFB7F-8249-4DC8-9334-19967328EA30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2412,8 +2558,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3248025" y="4257675"/>
-          <a:ext cx="323850" cy="352425"/>
+          <a:off x="3248025" y="4160520"/>
+          <a:ext cx="323850" cy="312420"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2473,7 +2619,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D03927-AD71-4363-8DEC-594E5D61AABA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D03927-AD71-4363-8DEC-594E5D61AABA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2523,7 +2669,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39864B6F-72B3-403A-9526-2069311F730F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39864B6F-72B3-403A-9526-2069311F730F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2587,7 +2733,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3289B93-5729-4860-B165-9AA9D37DA19D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3289B93-5729-4860-B165-9AA9D37DA19D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2651,7 +2797,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00CBF116-4490-46A5-A6F5-FA617976032F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00CBF116-4490-46A5-A6F5-FA617976032F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2720,7 +2866,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426CB00A-A4FE-48D3-8EC8-8E56481F709E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426CB00A-A4FE-48D3-8EC8-8E56481F709E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2770,7 +2916,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7139C1-3F1A-4A7B-BD39-6A4086C3049C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7139C1-3F1A-4A7B-BD39-6A4086C3049C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2834,7 +2980,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C3DE251-9B26-4626-B556-3867677B6D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C3DE251-9B26-4626-B556-3867677B6D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2898,7 +3044,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC09764-BC27-46A7-85BC-AF28131A32FD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DC09764-BC27-46A7-85BC-AF28131A32FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2962,7 +3108,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8600B3FE-4BB8-4365-B10F-534F48A254E0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8600B3FE-4BB8-4365-B10F-534F48A254E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3031,7 +3177,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FFF7F8F-52DF-49D0-B49E-FB1302B3AFA8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FFF7F8F-52DF-49D0-B49E-FB1302B3AFA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3081,7 +3227,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D702F8B7-D518-4B4B-89E4-E0AA9413A86D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D702F8B7-D518-4B4B-89E4-E0AA9413A86D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3145,7 +3291,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1B558AC-8429-43A0-9212-34BE12433C07}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1B558AC-8429-43A0-9212-34BE12433C07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3209,7 +3355,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE90FE44-8350-475A-ABFC-E23EB564F57E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE90FE44-8350-475A-ABFC-E23EB564F57E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3273,7 +3419,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E572BA-E1D9-438B-9092-CBF29A9AF2A1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7E572BA-E1D9-438B-9092-CBF29A9AF2A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3337,7 +3483,7 @@
         <xdr:cNvPr id="7" name="Oval 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB81CCC-A86E-4E47-A86E-7DDEEAEF062D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DB81CCC-A86E-4E47-A86E-7DDEEAEF062D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3406,7 +3552,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EDA7D5-5806-42E9-8844-BE3A0F6DA31D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EDA7D5-5806-42E9-8844-BE3A0F6DA31D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,7 +3602,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B40A96-A30C-49CD-9E55-F0083B39B860}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B40A96-A30C-49CD-9E55-F0083B39B860}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3520,7 +3666,7 @@
         <xdr:cNvPr id="4" name="Oval 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7399D90C-9BD6-4038-9D4A-89324A267051}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7399D90C-9BD6-4038-9D4A-89324A267051}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3584,7 +3730,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D988ED7-58C7-42AA-8E08-C9D3C6E28B5A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D988ED7-58C7-42AA-8E08-C9D3C6E28B5A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3648,7 +3794,7 @@
         <xdr:cNvPr id="6" name="Oval 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB0A4606-C187-4371-8ABE-941504EC046C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB0A4606-C187-4371-8ABE-941504EC046C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3712,7 +3858,7 @@
         <xdr:cNvPr id="7" name="Oval 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA3A66A4-CE27-414A-B10F-E401A5CB24F4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA3A66A4-CE27-414A-B10F-E401A5CB24F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3776,7 +3922,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB7F270B-2BCF-4664-AB08-2D21CC3771BE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB7F270B-2BCF-4664-AB08-2D21CC3771BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3840,7 +3986,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5991E4-C5FC-4E1F-AC8A-FF252EF603D9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5991E4-C5FC-4E1F-AC8A-FF252EF603D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3904,7 +4050,7 @@
         <xdr:cNvPr id="10" name="Oval 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E3BF1D-DFB6-4E26-9F7B-CF5B4F66817C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E3BF1D-DFB6-4E26-9F7B-CF5B4F66817C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3973,7 +4119,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F417FE2A-2BCC-45FC-A2A3-67E912870960}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F417FE2A-2BCC-45FC-A2A3-67E912870960}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4023,7 +4169,7 @@
         <xdr:cNvPr id="3" name="Oval 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F63D576-9CE4-401E-A99A-9BB2D51EDE52}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F63D576-9CE4-401E-A99A-9BB2D51EDE52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4087,7 +4233,7 @@
         <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DAC38F-CB4B-42F9-ACC7-2B7FB8D3500E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DAC38F-CB4B-42F9-ACC7-2B7FB8D3500E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4151,7 +4297,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46684365-4A9E-4DBF-9AB7-80D30D6399DD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46684365-4A9E-4DBF-9AB7-80D30D6399DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4215,7 +4361,7 @@
         <xdr:cNvPr id="9" name="Oval 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60425884-C4E9-4F5B-9F13-278776B6691C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60425884-C4E9-4F5B-9F13-278776B6691C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4279,7 +4425,7 @@
         <xdr:cNvPr id="10" name="Oval 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81D2274C-9732-46F0-8A44-986126A20879}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81D2274C-9732-46F0-8A44-986126A20879}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4343,7 +4489,7 @@
         <xdr:cNvPr id="11" name="Oval 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7E9EBBE-A169-484A-A090-85D3B71E4239}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7E9EBBE-A169-484A-A090-85D3B71E4239}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4681,7 +4827,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4690,15 +4836,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4706,7 +4852,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4717,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -4728,7 +4874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4738,8 +4884,14 @@
       <c r="H4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>145</v>
+      </c>
+      <c r="S4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4749,8 +4901,11 @@
       <c r="H5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4761,7 +4916,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4769,7 +4924,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4780,7 +4935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4788,7 +4943,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4799,7 +4954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4810,7 +4965,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4821,7 +4976,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4832,7 +4987,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4840,7 +4995,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4854,7 +5009,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4868,7 +5023,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4876,7 +5031,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4884,7 +5039,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4892,7 +5047,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4900,7 +5055,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4908,7 +5063,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -4916,7 +5071,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4924,7 +5079,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4932,7 +5087,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4940,7 +5095,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -4948,7 +5103,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -4956,7 +5111,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4964,7 +5119,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4972,7 +5127,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4980,7 +5135,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -4988,7 +5143,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -4996,7 +5151,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -5004,7 +5159,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -5012,7 +5167,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -5020,7 +5175,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -5028,7 +5183,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -5036,7 +5191,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -5053,18 +5208,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5072,7 +5227,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5083,7 +5238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5094,7 +5249,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5105,7 +5260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -5115,8 +5270,11 @@
       <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R5" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5126,16 +5284,22 @@
       <c r="H6" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="R7" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -5146,7 +5310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5157,7 +5321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5168,7 +5332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5176,7 +5340,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5187,7 +5351,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5198,7 +5362,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -5209,7 +5373,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5220,7 +5384,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -5231,7 +5395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5242,7 +5406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5250,7 +5414,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -5264,7 +5428,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5278,7 +5442,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5286,7 +5450,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5294,7 +5458,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5302,7 +5466,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5310,7 +5474,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5318,7 +5482,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5326,7 +5490,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5334,7 +5498,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5342,7 +5506,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5350,7 +5514,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5358,7 +5522,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5366,7 +5530,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5374,7 +5538,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5382,7 +5546,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5390,7 +5554,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5398,7 +5562,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5406,7 +5570,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5414,7 +5578,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5432,18 +5596,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5451,7 +5615,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5462,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5473,7 +5637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5483,8 +5647,11 @@
       <c r="H4" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R4" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -5494,8 +5661,14 @@
       <c r="H5" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5505,8 +5678,11 @@
       <c r="H6" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R6" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5516,8 +5692,17 @@
       <c r="H7" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -5527,8 +5712,11 @@
       <c r="H8" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R8" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5538,8 +5726,11 @@
       <c r="H9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R9" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5549,8 +5740,11 @@
       <c r="H10" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R10" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5560,8 +5754,11 @@
       <c r="H11" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R11" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5571,8 +5768,11 @@
       <c r="H12" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R12" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5582,16 +5782,22 @@
       <c r="H13" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R13" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="R14" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5601,8 +5807,11 @@
       <c r="H15" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R15" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -5613,7 +5822,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5624,7 +5833,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5635,7 +5844,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -5646,7 +5855,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5657,7 +5866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5668,7 +5877,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5679,7 +5888,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5690,7 +5899,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5701,7 +5910,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5709,7 +5918,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5720,7 +5929,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5731,7 +5940,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5742,7 +5951,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5753,7 +5962,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5764,7 +5973,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5775,7 +5984,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5786,7 +5995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5797,7 +6006,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5805,7 +6014,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5822,7 +6031,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5839,7 +6048,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5856,7 +6065,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5881,18 +6090,18 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5900,7 +6109,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5911,7 +6120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5922,7 +6131,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5932,8 +6141,11 @@
       <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R4" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -5943,8 +6155,14 @@
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5954,8 +6172,11 @@
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R6" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5965,8 +6186,17 @@
       <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -5976,8 +6206,11 @@
       <c r="H8" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R8" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5987,8 +6220,11 @@
       <c r="H9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R9" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5998,8 +6234,11 @@
       <c r="H10" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R10" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6009,16 +6248,22 @@
       <c r="H11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R11" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="R12" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6028,8 +6273,11 @@
       <c r="H13" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R13" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6040,7 +6288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6051,7 +6299,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6062,7 +6310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6073,7 +6321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6084,7 +6332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6095,7 +6343,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6106,7 +6354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6117,7 +6365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6125,7 +6373,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6136,7 +6384,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6147,7 +6395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6158,7 +6406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6169,7 +6417,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6180,7 +6428,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6191,7 +6439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6199,7 +6447,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6216,7 +6464,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6233,7 +6481,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6248,7 +6496,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6256,7 +6504,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6264,7 +6512,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6272,7 +6520,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6280,7 +6528,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6288,7 +6536,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6306,18 +6554,18 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6325,7 +6573,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6335,8 +6583,11 @@
       <c r="H2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q2" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6346,8 +6597,11 @@
       <c r="H3" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q3" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -6357,8 +6611,11 @@
       <c r="H4" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q4" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6369,7 +6626,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6377,7 +6634,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6388,7 +6645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -6396,7 +6653,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6407,7 +6664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6418,7 +6675,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6426,7 +6683,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6440,7 +6697,7 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6454,7 +6711,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6462,7 +6719,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6470,7 +6727,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6478,7 +6735,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6486,7 +6743,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6494,7 +6751,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6502,7 +6759,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6510,7 +6767,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6518,7 +6775,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6526,7 +6783,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6534,7 +6791,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6542,7 +6799,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6550,7 +6807,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6558,7 +6815,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6566,7 +6823,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6574,7 +6831,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6582,7 +6839,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6590,7 +6847,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6598,7 +6855,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6606,7 +6863,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6614,7 +6871,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6622,7 +6879,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6630,7 +6887,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6638,7 +6895,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6646,7 +6903,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6664,18 +6921,18 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6683,7 +6940,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6694,7 +6951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6704,8 +6961,11 @@
       <c r="H3" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q3" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -6715,8 +6975,11 @@
       <c r="H4" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q4" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6726,8 +6989,11 @@
       <c r="H5" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="Q5" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6738,7 +7004,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6746,7 +7012,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -6757,7 +7023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6765,7 +7031,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6776,7 +7042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6787,7 +7053,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6798,7 +7064,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6806,7 +7072,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6820,7 +7086,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6834,7 +7100,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6842,7 +7108,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6850,7 +7116,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6858,7 +7124,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6866,7 +7132,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6874,7 +7140,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6882,7 +7148,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6890,7 +7156,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6898,7 +7164,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6906,7 +7172,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6914,7 +7180,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6922,7 +7188,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6930,7 +7196,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6938,7 +7204,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6946,7 +7212,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6954,7 +7220,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6962,7 +7228,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6970,7 +7236,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6978,7 +7244,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6986,7 +7252,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6994,7 +7260,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7002,7 +7268,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7010,7 +7276,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -7028,18 +7294,18 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7047,7 +7313,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7058,7 +7324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -7069,7 +7335,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -7079,8 +7345,11 @@
       <c r="H4" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R4" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -7090,8 +7359,11 @@
       <c r="H5" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R5" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -7101,8 +7373,11 @@
       <c r="H6" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R6" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7112,8 +7387,11 @@
       <c r="H7" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="R7" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -7121,7 +7399,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7132,7 +7410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -7143,7 +7421,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -7151,7 +7429,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -7162,7 +7440,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -7173,7 +7451,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -7184,7 +7462,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -7195,7 +7473,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -7203,7 +7481,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -7217,7 +7495,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -7231,7 +7509,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -7245,7 +7523,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -7253,7 +7531,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -7261,7 +7539,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -7269,7 +7547,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -7277,7 +7555,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -7285,7 +7563,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -7293,7 +7571,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -7301,7 +7579,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -7309,7 +7587,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -7317,7 +7595,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -7325,7 +7603,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -7333,7 +7611,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -7341,7 +7619,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -7349,7 +7627,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -7357,7 +7635,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -7365,7 +7643,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -7373,7 +7651,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7381,7 +7659,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7389,7 +7667,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -7406,18 +7684,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7425,7 +7703,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7436,7 +7714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -7447,7 +7725,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -7458,7 +7736,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -7469,7 +7747,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -7479,8 +7757,11 @@
       <c r="H6" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R6" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7490,8 +7771,11 @@
       <c r="H7" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R7" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -7501,8 +7785,11 @@
       <c r="H8" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R8" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7512,8 +7799,11 @@
       <c r="H9" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R9" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -7523,16 +7813,22 @@
       <c r="H10" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R10" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="R11" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -7542,16 +7838,22 @@
       <c r="H12" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R12" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="R13" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -7561,8 +7863,11 @@
       <c r="H14" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R14" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -7572,8 +7877,11 @@
       <c r="H15" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R15" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -7584,15 +7892,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="R17" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -7605,8 +7916,11 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="R18" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -7620,7 +7934,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -7632,7 +7946,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -7640,7 +7954,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -7648,7 +7962,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -7656,7 +7970,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -7664,7 +7978,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -7672,7 +7986,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -7680,7 +7994,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -7688,7 +8002,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -7696,7 +8010,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -7704,7 +8018,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -7712,7 +8026,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -7720,7 +8034,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -7728,7 +8042,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -7736,7 +8050,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -7744,7 +8058,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -7752,7 +8066,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7760,7 +8074,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7768,7 +8082,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -7777,26 +8091,29 @@
       <c r="F38" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R13" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6:R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7804,7 +8121,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7815,7 +8132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -7826,7 +8143,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -7836,8 +8153,11 @@
       <c r="H4" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R4" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -7847,8 +8167,11 @@
       <c r="H5" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R5" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -7858,8 +8181,11 @@
       <c r="H6" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R6" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -7869,8 +8195,11 @@
       <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="R7" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -7881,7 +8210,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -7889,7 +8218,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -7900,7 +8229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -7908,7 +8237,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -7919,7 +8248,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -7930,7 +8259,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -7941,7 +8270,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -7949,7 +8278,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -7957,7 +8286,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -7971,7 +8300,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -7985,7 +8314,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -7993,7 +8322,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -8001,7 +8330,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -8009,7 +8338,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -8017,7 +8346,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8025,7 +8354,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -8033,7 +8362,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -8041,7 +8370,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -8049,7 +8378,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -8057,7 +8386,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -8065,7 +8394,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -8073,7 +8402,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -8081,7 +8410,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -8089,7 +8418,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -8097,7 +8426,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -8105,7 +8434,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -8113,7 +8442,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -8121,7 +8450,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -8129,7 +8458,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -8137,7 +8466,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>

</xml_diff>